<commit_message>
corrected a client typo
</commit_message>
<xml_diff>
--- a/apc/example_data/Holford1983Biometrics.xlsx
+++ b/apc/example_data/Holford1983Biometrics.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="84" windowWidth="22980" windowHeight="12960" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="90" windowWidth="22980" windowHeight="12960" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,9 +19,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
-    <t>Prostate Cancer Incidence, Nonwhites</t>
-  </si>
-  <si>
     <t>50 - 54</t>
   </si>
   <si>
@@ -86,6 +83,9 @@
   </si>
   <si>
     <t>Example from: Holford T.R. The estimation of age, period, and cohort effects for vital rates. Biometrics, 1983; 39:311-324.</t>
+  </si>
+  <si>
+    <t>Prostate Cancer Mortality, Nonwhites</t>
   </si>
 </sst>
 </file>
@@ -428,7 +428,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -440,7 +440,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -452,7 +452,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -462,80 +462,78 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="16.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="16" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.42578125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="16" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.44140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.42578125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="16" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16.44140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.42578125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="16" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="16.44140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="16.42578125" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
         <v>8</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>9</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>10</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>11</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>12</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>13</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>14</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>15</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>16</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>17</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
         <v>18</v>
       </c>
-      <c r="M2" t="s">
+      <c r="N2" t="s">
         <v>19</v>
       </c>
-      <c r="N2" t="s">
+      <c r="O2" t="s">
         <v>20</v>
-      </c>
-      <c r="O2" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B3">
         <v>177</v>
@@ -582,7 +580,7 @@
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B4">
         <v>262</v>
@@ -629,7 +627,7 @@
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B5">
         <v>360</v>
@@ -676,7 +674,7 @@
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B6">
         <v>409</v>
@@ -723,7 +721,7 @@
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B7">
         <v>328</v>
@@ -770,7 +768,7 @@
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B8">
         <v>222</v>
@@ -817,7 +815,7 @@
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B9">
         <v>108</v>
@@ -864,7 +862,7 @@
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>